<commit_message>
added rest of answer choices
</commit_message>
<xml_diff>
--- a/KahootBlank-JacTobias.xlsx
+++ b/KahootBlank-JacTobias.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\EXT\QC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3EAF074E-673F-4A92-B302-F84507C89947}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{822FB861-A40B-4244-8C89-19F2D0401CD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-20" yWindow="-530" windowWidth="19240" windowHeight="11490" tabRatio="338" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>Quiz template</t>
   </si>
@@ -126,6 +126,12 @@
   </si>
   <si>
     <t>1,3</t>
+  </si>
+  <si>
+    <t>To call the BusinessAccount print method instead of the Savings Account print method</t>
+  </si>
+  <si>
+    <t>To create the BusinessAccount class</t>
   </si>
 </sst>
 </file>
@@ -852,8 +858,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView tabSelected="1" topLeftCell="B2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1124,7 +1130,7 @@
       <c r="Z8" s="1"/>
       <c r="AA8" s="1"/>
     </row>
-    <row r="9" spans="1:27" ht="55.5" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:27" ht="92.5" x14ac:dyDescent="0.5">
       <c r="A9" s="11">
         <v>1</v>
       </c>
@@ -1140,7 +1146,9 @@
       <c r="E9" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="F9" s="14"/>
+      <c r="F9" s="14" t="s">
+        <v>31</v>
+      </c>
       <c r="G9" s="14">
         <v>10</v>
       </c>
@@ -1228,7 +1236,9 @@
       <c r="E11" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="F11" s="19"/>
+      <c r="F11" s="19" t="s">
+        <v>32</v>
+      </c>
       <c r="G11" s="19">
         <v>10</v>
       </c>

</xml_diff>